<commit_message>
Docs: Create .md files and add permissions
엑셀파일에 permissions column 추가 및 일부 api 수정
엑셀과 같은 내용의 Markdown 문서 생성
User 종류에 따른 권한 정리하여 Markdown 문서 생성 (#9)
</commit_message>
<xml_diff>
--- a/docs/studycafe_design.xlsx
+++ b/docs/studycafe_design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qaws1\Documents\DjangoProjects\studycafe_api\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03CBB43-E45C-42BA-8B14-044E6A049517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBB8974-6FB4-4CB1-9D00-0D40058FB04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{97F2C56D-309D-47A1-97CF-EFDC4E602C89}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="84">
   <si>
     <t>GET</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -347,6 +347,30 @@
   </si>
   <si>
     <t>user-update (email, student)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AllowAny</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsAdminUser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsAuthenticated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsOwner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsOwner | IsAdminUser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -354,7 +378,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -367,6 +391,22 @@
       <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -399,7 +439,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -410,6 +450,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -726,19 +772,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD0BB6A3-074F-429C-9AC8-7A7F985491C9}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="26.09765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="20.8984375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -746,393 +795,636 @@
         <v>72</v>
       </c>
       <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT(IF(ISTEXT(D2),"/"&amp;D2,""),IF(ISTEXT(E2),"/"&amp;E2,""),IF(ISTEXT(F2),"/"&amp;F2,""),IF(ISTEXT(G2),"/"&amp;G2,""))</f>
+        <v>/students</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="H2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C34" si="0">_xlfn.CONCAT(IF(ISTEXT(D3),"/"&amp;D3,""),IF(ISTEXT(E3),"/"&amp;E3,""),IF(ISTEXT(F3),"/"&amp;F3,""),IF(ISTEXT(G3),"/"&amp;G3,""))</f>
+        <v>/students/&lt;int:pk&gt;</v>
+      </c>
+      <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>/students/&lt;int:pk&gt;/purchases</v>
+      </c>
+      <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>/students/&lt;int:pk&gt;/rents/?year=2020&amp;month=4</v>
+      </c>
+      <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>/students/&lt;int:pk&gt;/ticket-storable</v>
+      </c>
+      <c r="D6" t="s">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A7" s="2" t="s">
+      <c r="H6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>/students/&lt;int:pk&gt;</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>49</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>/tickets</v>
+      </c>
+      <c r="D9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>50</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>/tickets/&lt;int:pk&gt;</v>
+      </c>
+      <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>55</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>/tickets</v>
+      </c>
+      <c r="D11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>51</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>/tickets/&lt;int:pk&gt;</v>
+      </c>
+      <c r="D12" t="s">
         <v>13</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>6</v>
       </c>
       <c r="H12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>58</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>/tickets/&lt;int:pk&gt;</v>
+      </c>
+      <c r="D13" t="s">
         <v>13</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>6</v>
       </c>
       <c r="H13" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>25</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>/seats</v>
+      </c>
+      <c r="D15" t="s">
         <v>15</v>
       </c>
       <c r="H15" t="s">
+        <v>78</v>
+      </c>
+      <c r="I15" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>24</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>/seats/?</v>
+      </c>
+      <c r="D16" t="s">
         <v>15</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>26</v>
       </c>
       <c r="H16" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>56</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>/seats</v>
+      </c>
+      <c r="D17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>57</v>
       </c>
       <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>/seats/&lt;int:pk&gt;</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
         <v>20</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>/seats/&lt;int:pk&gt;</v>
+      </c>
+      <c r="D19" t="s">
         <v>15</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E19" t="s">
         <v>6</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H19" t="s">
+        <v>79</v>
+      </c>
+      <c r="I19" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C20" t="str">
+        <f>_xlfn.CONCAT(IF(ISTEXT(D20),"/"&amp;D20,""),IF(ISTEXT(E20),"/"&amp;E20,""),IF(ISTEXT(F20),"/"&amp;F20,""),IF(ISTEXT(G20),"/"&amp;G20,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
         <v>63</v>
-      </c>
-      <c r="B20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>23</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>/purchases</v>
+      </c>
+      <c r="D21" t="s">
         <v>4</v>
       </c>
-      <c r="D21" t="s">
+      <c r="H21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>/purchases/price/?year=2020</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
         <v>17</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F22" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
+      <c r="H22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
         <v>64</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>7</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>/purchases</v>
+      </c>
+      <c r="D23" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
+      <c r="H23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
         <v>65</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>0</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>/rents</v>
+      </c>
+      <c r="D25" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
+      <c r="H25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
         <v>66</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>7</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>/rents</v>
+      </c>
+      <c r="D26" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
+      <c r="H26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
         <v>67</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>19</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>/rents</v>
+      </c>
+      <c r="D27" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A28" t="s">
+      <c r="H27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
         <v>21</v>
-      </c>
-      <c r="B28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
-        <v>22</v>
       </c>
       <c r="B29" t="s">
         <v>0</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>/users</v>
+      </c>
+      <c r="D29" t="s">
         <v>8</v>
       </c>
-      <c r="D29" t="s">
+      <c r="H29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>/users/&lt;int:pk&gt;</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
+      <c r="H30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
         <v>68</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>7</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>/users</v>
+      </c>
+      <c r="D31" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
+      <c r="H31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
         <v>77</v>
-      </c>
-      <c r="B31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>75</v>
       </c>
       <c r="B32" t="s">
         <v>19</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>/users/&lt;int:pk&gt;</v>
+      </c>
+      <c r="D32" t="s">
         <v>8</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>6</v>
       </c>
-      <c r="E32" t="s">
+      <c r="H32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>/users/&lt;int:pk&gt;/password</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A33" s="2" t="s">
+      <c r="H33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A34" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>20</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>/users/&lt;int:pk&gt;</v>
+      </c>
+      <c r="D34" t="s">
         <v>8</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E34" t="s">
         <v>6</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H34" t="s">
+        <v>81</v>
+      </c>
+      <c r="I34" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>